<commit_message>
prace na tray jako soucast aplikace - temer doreseno
</commit_message>
<xml_diff>
--- a/TRIMAZKON/dist/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/dist/config_TRIMAZKON.xlsx
@@ -603,12 +603,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>511_Teleflex</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>192.168.1.242</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -618,11 +618,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.??NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
+          <t xml:space="preserve">Teleflex </t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -632,12 +628,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -646,31 +642,6 @@
         </is>
       </c>
       <c r="D10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -686,19 +657,44 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -708,11 +704,15 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.??NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -770,9 +770,6 @@
       <c r="D14" t="inlineStr">
         <is>
           <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
 FH-2050-20
 10.96.205.80</t>
         </is>
@@ -931,12 +928,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -951,46 +948,56 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>xfdx</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>\\192.168.000.000\</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ss</t>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1000,7 +1007,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1015,89 +1022,84 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Druha sít, ixon</t>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1105,34 +1107,7 @@
           <t>*Jhv2708</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>10.96.205.166
 VisionNas_474B	
@@ -1142,9 +1117,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
@@ -1192,7 +1164,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1202,7 +1174,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1309,6 +1281,28 @@
       </c>
       <c r="E1" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>xfdx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\192.168.000.000\</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
automaticke ukladani historie cest, možnost smazání historie, upravy syntaxe
</commit_message>
<xml_diff>
--- a/TRIMAZKON/dist/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/dist/config_TRIMAZKON.xlsx
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -1174,7 +1174,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
práce na angličtině a menší úpravy
</commit_message>
<xml_diff>
--- a/TRIMAZKON/dist/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/dist/config_TRIMAZKON.xlsx
@@ -1774,14 +1774,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TRIMAZKON_task_1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>C:/Users/jakub.hlavacek.local/Desktop/JHV/test_images/Keyence/_503_Witte/datumovka/A/Height_test/</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>336</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>998</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>30.01.2025 10:03:29</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
prace na novem instaleru, aby neblokoval antivir
</commit_message>
<xml_diff>
--- a/TRIMAZKON/dist/config_TRIMAZKON.xlsx
+++ b/TRIMAZKON/dist/config_TRIMAZKON.xlsx
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ano</t>
+          <t>ne</t>
         </is>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1813,7 +1813,6 @@
           <t>30.01.2025 10:03:29</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>